<commit_message>
20190222 修改Bug 102 103 104 105
</commit_message>
<xml_diff>
--- a/templates/(舊報機單併X3)轉出關貿格式範例.xlsx
+++ b/templates/(舊報機單併X3)轉出關貿格式範例.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="10350" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="10356" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="NGIUOW" sheetId="5" state="veryHidden" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">快遞專區倉單         </t>
   </si>
@@ -140,10 +140,6 @@
   </si>
   <si>
     <t>${table:data.IL_GETADDRESS}</t>
-    <phoneticPr fontId="31" type="noConversion"/>
-  </si>
-  <si>
-    <t>${table:data.IL_TAX2}</t>
     <phoneticPr fontId="31" type="noConversion"/>
   </si>
   <si>
@@ -256,11 +252,23 @@
     <t>${table:data.IL_GETNAME_NEW}</t>
     <phoneticPr fontId="31" type="noConversion"/>
   </si>
+  <si>
+    <t>${table:data.IL_TAX2}</t>
+    <phoneticPr fontId="31" type="noConversion"/>
+  </si>
+  <si>
+    <t>匯出電話</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>${table:data.IL_EXTEL}</t>
+    <phoneticPr fontId="31" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="0_);[Red]\(0\)"/>
@@ -1071,7 +1079,21 @@
     <cellStyle name="警告文本" xfId="41"/>
     <cellStyle name="쉼표 [0] 10" xfId="42"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="32">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1588,7 +1610,7 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <sheetData/>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1605,26 +1627,27 @@
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="19.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="19.8"/>
   <cols>
     <col min="1" max="1" width="8.5" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="16.75" style="4" customWidth="1"/>
-    <col min="4" max="4" width="19.875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="7.75" style="5" customWidth="1"/>
+    <col min="2" max="2" width="13.09765625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="16.69921875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="19.8984375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="7.69921875" style="5" customWidth="1"/>
     <col min="6" max="6" width="7.5" style="5" customWidth="1"/>
     <col min="7" max="7" width="7" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.625" style="5" customWidth="1"/>
+    <col min="8" max="8" width="6.59765625" style="5" customWidth="1"/>
     <col min="9" max="9" width="7" style="5" customWidth="1"/>
     <col min="10" max="10" width="18" style="5" customWidth="1"/>
     <col min="11" max="11" width="11" style="6" customWidth="1"/>
-    <col min="12" max="12" width="16.25" style="7" customWidth="1"/>
-    <col min="13" max="13" width="58.25" style="8" customWidth="1"/>
-    <col min="14" max="14" width="12.625" style="8" customWidth="1"/>
-    <col min="15" max="15" width="11.125" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.19921875" style="7" customWidth="1"/>
+    <col min="13" max="13" width="58.19921875" style="8" customWidth="1"/>
+    <col min="14" max="14" width="12.59765625" style="8" customWidth="1"/>
+    <col min="15" max="15" width="11.09765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.3984375" style="3" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.5" style="3" customWidth="1"/>
-    <col min="18" max="16384" width="9" style="3"/>
+    <col min="18" max="18" width="24.8984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="33" customHeight="1">
@@ -1745,7 +1768,7 @@
         <v>10</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K4" s="19" t="s">
         <v>11</v>
@@ -1757,7 +1780,7 @@
         <v>13</v>
       </c>
       <c r="N4" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O4" s="29" t="s">
         <v>17</v>
@@ -1767,14 +1790,17 @@
       </c>
       <c r="Q4" s="22" t="s">
         <v>19</v>
+      </c>
+      <c r="R4" s="22" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="32" t="s">
         <v>33</v>
-      </c>
-      <c r="B5" s="32" t="s">
-        <v>34</v>
       </c>
       <c r="C5" s="30" t="s">
         <v>24</v>
@@ -1783,43 +1809,46 @@
         <v>25</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F5" s="30" t="s">
         <v>26</v>
       </c>
       <c r="G5" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="J5" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="30" t="s">
-        <v>38</v>
-      </c>
       <c r="L5" s="30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M5" s="30" t="s">
         <v>27</v>
       </c>
       <c r="N5" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O5" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="P5" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="P5" s="34" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q5" s="31" t="s">
-        <v>28</v>
+      <c r="Q5" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="R5" s="32" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1833,6 +1862,14 @@
   </mergeCells>
   <phoneticPr fontId="23" type="noConversion"/>
   <conditionalFormatting sqref="B5">
+    <cfRule type="expression" dxfId="31" priority="33">
+      <formula>$T5="特特貨"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="34">
+      <formula>$T5="普特貨"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
     <cfRule type="expression" dxfId="29" priority="31">
       <formula>$T5="特特貨"</formula>
     </cfRule>
@@ -1840,7 +1877,7 @@
       <formula>$T5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5">
+  <conditionalFormatting sqref="D5">
     <cfRule type="expression" dxfId="27" priority="29">
       <formula>$T5="特特貨"</formula>
     </cfRule>
@@ -1848,7 +1885,7 @@
       <formula>$T5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5">
+  <conditionalFormatting sqref="F5">
     <cfRule type="expression" dxfId="25" priority="27">
       <formula>$T5="特特貨"</formula>
     </cfRule>
@@ -1856,7 +1893,7 @@
       <formula>$T5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
+  <conditionalFormatting sqref="G5">
     <cfRule type="expression" dxfId="23" priority="25">
       <formula>$T5="特特貨"</formula>
     </cfRule>
@@ -1864,7 +1901,7 @@
       <formula>$T5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G5">
+  <conditionalFormatting sqref="H5">
     <cfRule type="expression" dxfId="21" priority="23">
       <formula>$T5="特特貨"</formula>
     </cfRule>
@@ -1872,7 +1909,7 @@
       <formula>$T5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5">
+  <conditionalFormatting sqref="I5">
     <cfRule type="expression" dxfId="19" priority="21">
       <formula>$T5="特特貨"</formula>
     </cfRule>
@@ -1880,7 +1917,7 @@
       <formula>$T5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5">
+  <conditionalFormatting sqref="J5">
     <cfRule type="expression" dxfId="17" priority="19">
       <formula>$T5="特特貨"</formula>
     </cfRule>
@@ -1888,7 +1925,7 @@
       <formula>$T5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J5">
+  <conditionalFormatting sqref="K5">
     <cfRule type="expression" dxfId="15" priority="17">
       <formula>$T5="特特貨"</formula>
     </cfRule>
@@ -1896,7 +1933,7 @@
       <formula>$T5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K5">
+  <conditionalFormatting sqref="L5">
     <cfRule type="expression" dxfId="13" priority="15">
       <formula>$T5="特特貨"</formula>
     </cfRule>
@@ -1904,7 +1941,7 @@
       <formula>$T5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L5">
+  <conditionalFormatting sqref="M5">
     <cfRule type="expression" dxfId="11" priority="13">
       <formula>$T5="特特貨"</formula>
     </cfRule>
@@ -1912,15 +1949,15 @@
       <formula>$T5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M5">
+  <conditionalFormatting sqref="N5">
     <cfRule type="expression" dxfId="9" priority="11">
-      <formula>$T5="特特貨"</formula>
+      <formula>$S5="特特貨"</formula>
     </cfRule>
     <cfRule type="expression" dxfId="8" priority="12">
-      <formula>$T5="普特貨"</formula>
+      <formula>$S5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N5">
+  <conditionalFormatting sqref="O5">
     <cfRule type="expression" dxfId="7" priority="9">
       <formula>$S5="特特貨"</formula>
     </cfRule>
@@ -1928,15 +1965,15 @@
       <formula>$S5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O5">
-    <cfRule type="expression" dxfId="5" priority="7">
+  <conditionalFormatting sqref="Q5">
+    <cfRule type="expression" dxfId="5" priority="5">
       <formula>$S5="特特貨"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>$S5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q5">
+  <conditionalFormatting sqref="E5">
     <cfRule type="expression" dxfId="3" priority="3">
       <formula>$S5="特特貨"</formula>
     </cfRule>
@@ -1944,7 +1981,7 @@
       <formula>$S5="普特貨"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
+  <conditionalFormatting sqref="R5">
     <cfRule type="expression" dxfId="1" priority="1">
       <formula>$S5="特特貨"</formula>
     </cfRule>

</xml_diff>